<commit_message>
continued work on pipeline
</commit_message>
<xml_diff>
--- a/metadata_files/chemical_metadata.xlsx
+++ b/metadata_files/chemical_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34C66A9-EED0-8B48-83AE-5594F8B80A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB22E0F-3E5F-564C-AAC5-72F3F9AADB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="38400" windowHeight="19440" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
   </bookViews>
@@ -11704,9 +11704,6 @@
     <t>OD-PABA</t>
   </si>
   <si>
-    <t>58817-05-3</t>
-  </si>
-  <si>
     <t>Octyl-dimethyl-p-aminobenzoic acid</t>
   </si>
   <si>
@@ -11753,6 +11750,9 @@
   </si>
   <si>
     <t>Wood Preservativesᶜ</t>
+  </si>
+  <si>
+    <t>21245-02-3</t>
   </si>
 </sst>
 </file>
@@ -12293,8 +12293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CEBC29-3567-B44B-81AE-C9A53B403E66}">
   <dimension ref="A1:AD444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P437" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W282" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12754,7 +12754,7 @@
         <v>3879</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3895</v>
+        <v>3894</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2762</v>
@@ -12805,7 +12805,7 @@
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>685</v>
@@ -12834,7 +12834,7 @@
         <v>3880</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2762</v>
@@ -12887,7 +12887,7 @@
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>685</v>
@@ -12916,7 +12916,7 @@
         <v>3881</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2762</v>
@@ -12969,7 +12969,7 @@
       </c>
       <c r="V8" s="2"/>
       <c r="W8" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>685</v>
@@ -13047,7 +13047,7 @@
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>92</v>
@@ -13369,7 +13369,7 @@
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>122</v>
@@ -14479,7 +14479,7 @@
       </c>
       <c r="V27" s="2"/>
       <c r="W27" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X27" s="2" t="s">
         <v>312</v>
@@ -15449,7 +15449,7 @@
       </c>
       <c r="V39" s="2"/>
       <c r="W39" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X39" s="2" t="s">
         <v>217</v>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="V40" s="2"/>
       <c r="W40" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>92</v>
@@ -15845,7 +15845,7 @@
       </c>
       <c r="V44" s="2"/>
       <c r="W44" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X44" s="2" t="s">
         <v>122</v>
@@ -16247,7 +16247,7 @@
       </c>
       <c r="V49" s="2"/>
       <c r="W49" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X49" s="2" t="s">
         <v>217</v>
@@ -16327,7 +16327,7 @@
       </c>
       <c r="V50" s="2"/>
       <c r="W50" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X50" s="2" t="s">
         <v>92</v>
@@ -16485,7 +16485,7 @@
       </c>
       <c r="V52" s="2"/>
       <c r="W52" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X52" s="2" t="s">
         <v>122</v>
@@ -17119,7 +17119,7 @@
       </c>
       <c r="V60" s="2"/>
       <c r="W60" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X60" s="2" t="s">
         <v>122</v>
@@ -17505,7 +17505,7 @@
       </c>
       <c r="V65" s="2"/>
       <c r="W65" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X65" s="2" t="s">
         <v>122</v>
@@ -17688,7 +17688,7 @@
         <v>864</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>863</v>
@@ -17739,7 +17739,7 @@
       </c>
       <c r="V68" s="2"/>
       <c r="W68" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X68" s="2" t="s">
         <v>92</v>
@@ -18363,7 +18363,7 @@
       </c>
       <c r="V76" s="2"/>
       <c r="W76" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X76" s="2" t="s">
         <v>92</v>
@@ -18443,7 +18443,7 @@
       </c>
       <c r="V77" s="2"/>
       <c r="W77" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X77" s="2" t="s">
         <v>122</v>
@@ -18527,7 +18527,7 @@
       </c>
       <c r="V78" s="2"/>
       <c r="W78" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X78" s="2" t="s">
         <v>92</v>
@@ -18689,7 +18689,7 @@
       </c>
       <c r="V80" s="2"/>
       <c r="W80" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X80" s="2" t="s">
         <v>92</v>
@@ -18925,7 +18925,7 @@
       </c>
       <c r="V83" s="2"/>
       <c r="W83" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X83" s="2" t="s">
         <v>92</v>
@@ -19007,7 +19007,7 @@
       </c>
       <c r="V84" s="2"/>
       <c r="W84" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X84" s="2" t="s">
         <v>92</v>
@@ -19245,7 +19245,7 @@
       </c>
       <c r="V87" s="2"/>
       <c r="W87" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X87" s="2" t="s">
         <v>312</v>
@@ -19407,7 +19407,7 @@
       </c>
       <c r="V89" s="2"/>
       <c r="W89" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X89" s="2" t="s">
         <v>92</v>
@@ -19647,7 +19647,7 @@
         <v>762</v>
       </c>
       <c r="W92" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X92" s="2" t="s">
         <v>312</v>
@@ -19727,7 +19727,7 @@
         <v>762</v>
       </c>
       <c r="W93" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X93" s="2" t="s">
         <v>312</v>
@@ -20205,7 +20205,7 @@
       </c>
       <c r="V99" s="2"/>
       <c r="W99" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X99" s="2" t="s">
         <v>312</v>
@@ -20753,7 +20753,7 @@
       </c>
       <c r="V106" s="2"/>
       <c r="W106" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X106" s="2" t="s">
         <v>92</v>
@@ -20833,7 +20833,7 @@
       </c>
       <c r="V107" s="2"/>
       <c r="W107" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X107" s="2" t="s">
         <v>217</v>
@@ -20911,7 +20911,7 @@
       </c>
       <c r="V108" s="2"/>
       <c r="W108" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X108" s="2" t="s">
         <v>312</v>
@@ -21777,7 +21777,7 @@
       </c>
       <c r="V119" s="2"/>
       <c r="W119" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X119" s="2" t="s">
         <v>217</v>
@@ -21857,7 +21857,7 @@
       </c>
       <c r="V120" s="2"/>
       <c r="W120" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X120" s="2" t="s">
         <v>92</v>
@@ -21935,7 +21935,7 @@
       </c>
       <c r="V121" s="2"/>
       <c r="W121" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X121" s="2" t="s">
         <v>217</v>
@@ -22017,7 +22017,7 @@
       </c>
       <c r="V122" s="2"/>
       <c r="W122" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X122" s="2" t="s">
         <v>312</v>
@@ -22413,7 +22413,7 @@
       </c>
       <c r="V127" s="2"/>
       <c r="W127" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X127" s="2" t="s">
         <v>92</v>
@@ -22491,7 +22491,7 @@
       </c>
       <c r="V128" s="2"/>
       <c r="W128" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X128" s="2" t="s">
         <v>122</v>
@@ -22965,7 +22965,7 @@
       </c>
       <c r="V134" s="2"/>
       <c r="W134" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X134" s="2" t="s">
         <v>92</v>
@@ -23043,7 +23043,7 @@
       </c>
       <c r="V135" s="2"/>
       <c r="W135" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X135" s="2" t="s">
         <v>217</v>
@@ -23199,7 +23199,7 @@
       </c>
       <c r="V137" s="2"/>
       <c r="W137" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X137" s="2" t="s">
         <v>312</v>
@@ -23430,12 +23430,12 @@
         <v>125</v>
       </c>
       <c r="T140" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
       <c r="W140" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="X140" s="2" t="s">
         <v>92</v>
@@ -24227,7 +24227,7 @@
       </c>
       <c r="V150" s="2"/>
       <c r="W150" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X150" s="2" t="s">
         <v>122</v>
@@ -25099,7 +25099,7 @@
       </c>
       <c r="V161" s="2"/>
       <c r="W161" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X161" s="2" t="s">
         <v>312</v>
@@ -25179,7 +25179,7 @@
       </c>
       <c r="V162" s="2"/>
       <c r="W162" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X162" s="2" t="s">
         <v>92</v>
@@ -25259,7 +25259,7 @@
       </c>
       <c r="V163" s="2"/>
       <c r="W163" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X163" s="2" t="s">
         <v>92</v>
@@ -25339,7 +25339,7 @@
       </c>
       <c r="V164" s="2"/>
       <c r="W164" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X164" s="2" t="s">
         <v>92</v>
@@ -26841,7 +26841,7 @@
       </c>
       <c r="V183" s="2"/>
       <c r="W183" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X183" s="2" t="s">
         <v>217</v>
@@ -26921,7 +26921,7 @@
       </c>
       <c r="V184" s="2"/>
       <c r="W184" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X184" s="2" t="s">
         <v>122</v>
@@ -27309,7 +27309,7 @@
       </c>
       <c r="V189" s="2"/>
       <c r="W189" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X189" s="2" t="s">
         <v>92</v>
@@ -27389,7 +27389,7 @@
       </c>
       <c r="V190" s="2"/>
       <c r="W190" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X190" s="2" t="s">
         <v>217</v>
@@ -27415,7 +27415,7 @@
         <v>105</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>3891</v>
+        <v>3890</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>2320</v>
@@ -27645,10 +27645,10 @@
         <v>105</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>3466</v>
@@ -27779,7 +27779,7 @@
       </c>
       <c r="V195" s="2"/>
       <c r="W195" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X195" s="2" t="s">
         <v>685</v>
@@ -27939,7 +27939,7 @@
       </c>
       <c r="V197" s="2"/>
       <c r="W197" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X197" s="2" t="s">
         <v>875</v>
@@ -28093,7 +28093,7 @@
       </c>
       <c r="V199" s="2"/>
       <c r="W199" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X199" s="2" t="s">
         <v>92</v>
@@ -28959,7 +28959,7 @@
       </c>
       <c r="V210" s="2"/>
       <c r="W210" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X210" s="2" t="s">
         <v>92</v>
@@ -29113,7 +29113,7 @@
       </c>
       <c r="V212" s="2"/>
       <c r="W212" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X212" s="2" t="s">
         <v>122</v>
@@ -29825,7 +29825,7 @@
       </c>
       <c r="V221" s="2"/>
       <c r="W221" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X221" s="2" t="s">
         <v>217</v>
@@ -30449,7 +30449,7 @@
       </c>
       <c r="V229" s="2"/>
       <c r="W229" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X229" s="2" t="s">
         <v>312</v>
@@ -30761,7 +30761,7 @@
       </c>
       <c r="V233" s="2"/>
       <c r="W233" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X233" s="2" t="s">
         <v>312</v>
@@ -31457,7 +31457,7 @@
       </c>
       <c r="V242" s="2"/>
       <c r="W242" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X242" s="2" t="s">
         <v>312</v>
@@ -31539,7 +31539,7 @@
       </c>
       <c r="V243" s="2"/>
       <c r="W243" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X243" s="2" t="s">
         <v>312</v>
@@ -32011,7 +32011,7 @@
       </c>
       <c r="V249" s="2"/>
       <c r="W249" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X249" s="2" t="s">
         <v>92</v>
@@ -32089,7 +32089,7 @@
       </c>
       <c r="V250" s="2"/>
       <c r="W250" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X250" s="2" t="s">
         <v>122</v>
@@ -32247,7 +32247,7 @@
       </c>
       <c r="V252" s="2"/>
       <c r="W252" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X252" s="2" t="s">
         <v>122</v>
@@ -32635,7 +32635,7 @@
       </c>
       <c r="V257" s="2"/>
       <c r="W257" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X257" s="2" t="s">
         <v>312</v>
@@ -32953,7 +32953,7 @@
       </c>
       <c r="V261" s="2"/>
       <c r="W261" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X261" s="2" t="s">
         <v>312</v>
@@ -33261,7 +33261,7 @@
         <v>1940</v>
       </c>
       <c r="W265" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X265" s="2" t="s">
         <v>239</v>
@@ -33339,7 +33339,7 @@
       </c>
       <c r="V266" s="2"/>
       <c r="W266" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X266" s="2" t="s">
         <v>122</v>
@@ -33423,7 +33423,7 @@
       </c>
       <c r="V267" s="2"/>
       <c r="W267" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X267" s="2" t="s">
         <v>122</v>
@@ -33581,7 +33581,7 @@
       </c>
       <c r="V269" s="2"/>
       <c r="W269" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X269" s="2" t="s">
         <v>92</v>
@@ -34363,7 +34363,7 @@
       </c>
       <c r="V279" s="2"/>
       <c r="W279" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X279" s="2" t="s">
         <v>312</v>
@@ -34443,7 +34443,7 @@
       </c>
       <c r="V280" s="2"/>
       <c r="W280" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X280" s="2" t="s">
         <v>122</v>
@@ -34601,7 +34601,7 @@
         <v>866</v>
       </c>
       <c r="W282" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X282" s="2" t="s">
         <v>122</v>
@@ -34759,7 +34759,7 @@
       <c r="U284" s="2"/>
       <c r="V284" s="2"/>
       <c r="W284" s="3" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="X284" s="2" t="s">
         <v>92</v>
@@ -35146,12 +35146,12 @@
         <v>125</v>
       </c>
       <c r="T289" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="U289" s="2"/>
       <c r="V289" s="2"/>
       <c r="W289" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="X289" s="2" t="s">
         <v>92</v>
@@ -35231,7 +35231,7 @@
       </c>
       <c r="V290" s="2"/>
       <c r="W290" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X290" s="2" t="s">
         <v>92</v>
@@ -35471,7 +35471,7 @@
       </c>
       <c r="V293" s="2"/>
       <c r="W293" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X293" s="2" t="s">
         <v>312</v>
@@ -35627,7 +35627,7 @@
       <c r="U295" s="3"/>
       <c r="V295" s="3"/>
       <c r="W295" s="3" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="X295" s="2" t="s">
         <v>92</v>
@@ -35951,7 +35951,7 @@
       </c>
       <c r="V299" s="2"/>
       <c r="W299" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X299" s="2" t="s">
         <v>122</v>
@@ -36187,7 +36187,7 @@
       </c>
       <c r="V302" s="2"/>
       <c r="W302" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X302" s="2" t="s">
         <v>602</v>
@@ -36265,7 +36265,7 @@
         <v>727</v>
       </c>
       <c r="W303" s="3" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="X303" s="2" t="s">
         <v>92</v>
@@ -36343,7 +36343,7 @@
       </c>
       <c r="V304" s="2"/>
       <c r="W304" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X304" s="2" t="s">
         <v>92</v>
@@ -36425,7 +36425,7 @@
       </c>
       <c r="V305" s="2"/>
       <c r="W305" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X305" s="2" t="s">
         <v>217</v>
@@ -36501,7 +36501,7 @@
       </c>
       <c r="V306" s="2"/>
       <c r="W306" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X306" s="2" t="s">
         <v>92</v>
@@ -37049,7 +37049,7 @@
       </c>
       <c r="V313" s="2"/>
       <c r="W313" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X313" s="2" t="s">
         <v>92</v>
@@ -37075,7 +37075,7 @@
         <v>1</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>3883</v>
@@ -37084,10 +37084,10 @@
         <v>2382</v>
       </c>
       <c r="F314" s="2" t="s">
-        <v>3884</v>
+        <v>3900</v>
       </c>
       <c r="G314" s="2">
-        <v>42851</v>
+        <v>30541</v>
       </c>
       <c r="H314" s="2" t="s">
         <v>2381</v>
@@ -37281,7 +37281,7 @@
       </c>
       <c r="V316" s="2"/>
       <c r="W316" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X316" s="2" t="s">
         <v>122</v>
@@ -37515,7 +37515,7 @@
       </c>
       <c r="V319" s="2"/>
       <c r="W319" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X319" s="2" t="s">
         <v>217</v>
@@ -38467,7 +38467,7 @@
       </c>
       <c r="V331" s="2"/>
       <c r="W331" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X331" s="2" t="s">
         <v>92</v>
@@ -39485,7 +39485,7 @@
       </c>
       <c r="V344" s="2"/>
       <c r="W344" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X344" s="2" t="s">
         <v>92</v>
@@ -39565,7 +39565,7 @@
       </c>
       <c r="V345" s="2"/>
       <c r="W345" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X345" s="2" t="s">
         <v>92</v>
@@ -39721,7 +39721,7 @@
       </c>
       <c r="V347" s="2"/>
       <c r="W347" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X347" s="2" t="s">
         <v>92</v>
@@ -39799,7 +39799,7 @@
       </c>
       <c r="V348" s="2"/>
       <c r="W348" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X348" s="2" t="s">
         <v>92</v>
@@ -39877,7 +39877,7 @@
       </c>
       <c r="V349" s="2"/>
       <c r="W349" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X349" s="2" t="s">
         <v>92</v>
@@ -40191,7 +40191,7 @@
       <c r="U353" s="3"/>
       <c r="V353" s="3"/>
       <c r="W353" s="3" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="X353" s="2" t="s">
         <v>92</v>
@@ -40273,7 +40273,7 @@
       <c r="U354" s="3"/>
       <c r="V354" s="3"/>
       <c r="W354" s="3" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="X354" s="2" t="s">
         <v>92</v>
@@ -40433,7 +40433,7 @@
       </c>
       <c r="V356" s="2"/>
       <c r="W356" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X356" s="2" t="s">
         <v>92</v>
@@ -40513,7 +40513,7 @@
       </c>
       <c r="V357" s="2"/>
       <c r="W357" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X357" s="2" t="s">
         <v>92</v>
@@ -41141,7 +41141,7 @@
       </c>
       <c r="V365" s="2"/>
       <c r="W365" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X365" s="2" t="s">
         <v>92</v>
@@ -41461,7 +41461,7 @@
       </c>
       <c r="V369" s="2"/>
       <c r="W369" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X369" s="2" t="s">
         <v>92</v>
@@ -41539,7 +41539,7 @@
       </c>
       <c r="V370" s="2"/>
       <c r="W370" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X370" s="2" t="s">
         <v>92</v>
@@ -41721,7 +41721,7 @@
         <v>105</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>133</v>
@@ -42011,7 +42011,7 @@
       </c>
       <c r="V376" s="2"/>
       <c r="W376" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X376" s="2" t="s">
         <v>92</v>
@@ -42784,12 +42784,12 @@
         <v>125</v>
       </c>
       <c r="T386" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="U386" s="2"/>
       <c r="V386" s="2"/>
       <c r="W386" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="X386" s="2" t="s">
         <v>92</v>
@@ -42813,7 +42813,7 @@
         <v>105</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>3897</v>
+        <v>3896</v>
       </c>
       <c r="D387" s="2" t="s">
         <v>856</v>
@@ -43171,7 +43171,7 @@
       </c>
       <c r="V391" s="2"/>
       <c r="W391" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X391" s="2" t="s">
         <v>92</v>
@@ -43325,7 +43325,7 @@
       </c>
       <c r="V393" s="2"/>
       <c r="W393" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X393" s="2" t="s">
         <v>92</v>
@@ -43407,7 +43407,7 @@
       </c>
       <c r="V394" s="2"/>
       <c r="W394" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X394" s="2" t="s">
         <v>92</v>
@@ -43560,12 +43560,12 @@
         <v>125</v>
       </c>
       <c r="T396" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="U396" s="2"/>
       <c r="V396" s="2"/>
       <c r="W396" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="X396" s="2" t="s">
         <v>92</v>
@@ -43795,7 +43795,7 @@
         <v>866</v>
       </c>
       <c r="W399" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X399" s="2" t="s">
         <v>122</v>
@@ -44029,7 +44029,7 @@
       </c>
       <c r="V402" s="2"/>
       <c r="W402" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X402" s="2" t="s">
         <v>92</v>
@@ -44107,7 +44107,7 @@
       </c>
       <c r="V403" s="2"/>
       <c r="W403" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X403" s="2" t="s">
         <v>92</v>
@@ -44505,7 +44505,7 @@
       </c>
       <c r="V408" s="2"/>
       <c r="W408" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X408" s="2" t="s">
         <v>122</v>
@@ -44745,7 +44745,7 @@
       </c>
       <c r="V411" s="2"/>
       <c r="W411" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X411" s="2" t="s">
         <v>122</v>
@@ -44911,7 +44911,7 @@
       </c>
       <c r="V413" s="3"/>
       <c r="W413" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X413" s="2" t="s">
         <v>122</v>
@@ -45299,7 +45299,7 @@
       </c>
       <c r="V418" s="2"/>
       <c r="W418" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X418" s="2" t="s">
         <v>92</v>
@@ -45531,7 +45531,7 @@
       </c>
       <c r="V421" s="2"/>
       <c r="W421" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X421" s="2" t="s">
         <v>122</v>
@@ -45929,7 +45929,7 @@
       </c>
       <c r="V426" s="2"/>
       <c r="W426" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X426" s="2" t="s">
         <v>92</v>
@@ -46035,7 +46035,7 @@
         <v>105</v>
       </c>
       <c r="C428" s="2" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="D428" s="2" t="s">
         <v>158</v>
@@ -46325,7 +46325,7 @@
       </c>
       <c r="V431" s="2"/>
       <c r="W431" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X431" s="2" t="s">
         <v>92</v>
@@ -46508,7 +46508,7 @@
         <v>1053</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="E434" s="2" t="s">
         <v>1052</v>
@@ -46557,7 +46557,7 @@
       </c>
       <c r="V434" s="2"/>
       <c r="W434" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="X434" s="2" t="s">
         <v>92</v>
@@ -46943,7 +46943,7 @@
       </c>
       <c r="V439" s="2"/>
       <c r="W439" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X439" s="2" t="s">
         <v>122</v>
@@ -46972,7 +46972,7 @@
         <v>2253</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="E440" s="2" t="s">
         <v>2252</v>
@@ -47097,7 +47097,7 @@
       </c>
       <c r="V441" s="2"/>
       <c r="W441" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="X441" s="2" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
worked on making manual validation export
</commit_message>
<xml_diff>
--- a/metadata_files/chemical_metadata.xlsx
+++ b/metadata_files/chemical_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFC45CE-775B-8E4F-A974-15D0832D6030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A85FE9-407C-264B-A552-0B8CB993513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="500" windowWidth="37260" windowHeight="19580" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="37260" windowHeight="19580" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_metadata" sheetId="30" r:id="rId1"/>
@@ -12296,8 +12296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CEBC29-3567-B44B-81AE-C9A53B403E66}">
   <dimension ref="A1:AD444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T344" sqref="T344"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W9" sqref="E9:W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>